<commit_message>
clean up mapping spreadsheet
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Query_Results_Service/artifacts/service_model/information_model/Court_Case_Query_Results-IEPD/documentation/Court_Case_Query_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Query_Results_Service/artifacts/service_model/information_model/Court_Case_Query_Results-IEPD/documentation/Court_Case_Query_Results-Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="25960" yWindow="-1720" windowWidth="29500" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -5749,16 +5749,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J309"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" style="18" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="18" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="73.1640625" style="18" customWidth="1"/>
     <col min="5" max="5" width="15" style="18" customWidth="1"/>
     <col min="6" max="6" width="22.5" style="18" customWidth="1"/>

</xml_diff>

<commit_message>
Changes "StateID" to "FingerprintID".
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Query_Results_Service/artifacts/service_model/information_model/Court_Case_Query_Results-IEPD/documentation/Court_Case_Query_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/service-specifications/Court_Case_Query_Results_Service/artifacts/service_model/information_model/Court_Case_Query_Results-IEPD/documentation/Court_Case_Query_Results-Mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="0" windowWidth="29500" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="5180" yWindow="1220" windowWidth="29500" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Query Results Mappin" sheetId="1" r:id="rId1"/>
@@ -3108,9 +3108,6 @@
     <t>ccq-res-doc:CourtCaseQueryResults/j:AppellateCase/nc:CaseTrackingID</t>
   </si>
   <si>
-    <t>ccq-res-doc:CourtCaseQueryResults/nc:Person/nc:PersonStateIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
     <t>ccq-res-doc:CourtCaseQueryResults/nc:Person/nc:PersonSSNIdentification/nc:IdentificationID</t>
   </si>
   <si>
@@ -3593,6 +3590,9 @@
   </si>
   <si>
     <t>not used</t>
+  </si>
+  <si>
+    <t>ccq-res-doc:CourtCaseQueryResults/nc:Person/j:PersonAugmentation/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
@@ -5784,8 +5784,8 @@
   <dimension ref="A1:J309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A295" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B305" sqref="B305"/>
+      <pane ySplit="2" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5837,7 +5837,7 @@
         <v>436</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -5896,7 +5896,7 @@
         <v>459</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -5955,7 +5955,7 @@
         <v>435</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -6470,7 +6470,7 @@
         <v>437</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -6548,7 +6548,7 @@
         <v>438</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -6615,7 +6615,7 @@
         <v>156</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -6651,7 +6651,7 @@
         <v>442</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
@@ -6687,7 +6687,7 @@
         <v>440</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -6742,7 +6742,7 @@
         <v>439</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
@@ -6958,7 +6958,7 @@
         <v>447</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
@@ -7191,10 +7191,10 @@
     </row>
     <row r="68" spans="1:7" ht="28">
       <c r="A68" s="15" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B68" s="15" t="s">
         <v>1173</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>1174</v>
       </c>
       <c r="C68" s="20" t="s">
         <v>464</v>
@@ -7217,7 +7217,7 @@
         <v>448</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
@@ -7233,7 +7233,7 @@
         <v>84</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D70" s="56"/>
       <c r="E70" s="55"/>
@@ -7251,7 +7251,7 @@
         <v>464</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>592</v>
@@ -7274,7 +7274,7 @@
         <v>464</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>592</v>
@@ -7297,7 +7297,7 @@
         <v>464</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>592</v>
@@ -7320,7 +7320,7 @@
         <v>464</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>592</v>
@@ -7343,7 +7343,7 @@
         <v>464</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="E75" s="4" t="s">
         <v>592</v>
@@ -7366,7 +7366,7 @@
         <v>464</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E76" s="4" t="s">
         <v>592</v>
@@ -7383,7 +7383,7 @@
         <v>449</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C77" s="12"/>
       <c r="D77" s="12"/>
@@ -7532,7 +7532,7 @@
         <v>441</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
@@ -7568,7 +7568,7 @@
         <v>458</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
@@ -7650,7 +7650,7 @@
         <v>460</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
@@ -7709,7 +7709,7 @@
         <v>624</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
@@ -7819,7 +7819,7 @@
         <v>443</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
@@ -7832,7 +7832,7 @@
         <v>199</v>
       </c>
       <c r="B100" s="59" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C100" s="48"/>
       <c r="D100" s="48"/>
@@ -7840,10 +7840,10 @@
         <v>565</v>
       </c>
       <c r="F100" s="55" t="s">
+        <v>1176</v>
+      </c>
+      <c r="G100" s="55" t="s">
         <v>1177</v>
-      </c>
-      <c r="G100" s="55" t="s">
-        <v>1178</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="28">
@@ -7866,13 +7866,13 @@
         <v>193</v>
       </c>
       <c r="B102" s="49" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C102" s="49" t="s">
         <v>464</v>
       </c>
       <c r="D102" s="58" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="E102" s="49" t="s">
         <v>548</v>
@@ -7884,7 +7884,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="30">
+    <row r="103" spans="1:7" ht="45">
       <c r="A103" s="49" t="s">
         <v>44</v>
       </c>
@@ -7895,7 +7895,7 @@
         <v>464</v>
       </c>
       <c r="D103" s="49" t="s">
-        <v>1029</v>
+        <v>1189</v>
       </c>
       <c r="E103" s="49" t="s">
         <v>565</v>
@@ -7918,7 +7918,7 @@
         <v>464</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E104" s="4" t="s">
         <v>565</v>
@@ -7941,7 +7941,7 @@
         <v>464</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>565</v>
@@ -7964,7 +7964,7 @@
         <v>464</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E106" s="4" t="s">
         <v>565</v>
@@ -7987,7 +7987,7 @@
         <v>464</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>565</v>
@@ -8010,7 +8010,7 @@
         <v>464</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E108" s="4" t="s">
         <v>565</v>
@@ -8033,7 +8033,7 @@
         <v>464</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>565</v>
@@ -8050,13 +8050,13 @@
         <v>196</v>
       </c>
       <c r="B110" s="4" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D110" s="2" t="s">
         <v>1036</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>1037</v>
       </c>
       <c r="E110" s="4" t="s">
         <v>565</v>
@@ -8079,7 +8079,7 @@
         <v>464</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E111" s="4" t="s">
         <v>565</v>
@@ -8102,7 +8102,7 @@
         <v>464</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E112" s="4" t="s">
         <v>565</v>
@@ -8125,7 +8125,7 @@
         <v>464</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>565</v>
@@ -8148,7 +8148,7 @@
         <v>464</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="E114" s="4" t="s">
         <v>565</v>
@@ -8169,7 +8169,7 @@
       </c>
       <c r="C115" s="28"/>
       <c r="D115" s="2" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="E115" s="4" t="s">
         <v>565</v>
@@ -8192,7 +8192,7 @@
         <v>464</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E116" s="4" t="s">
         <v>565</v>
@@ -8215,7 +8215,7 @@
         <v>464</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>565</v>
@@ -8259,7 +8259,7 @@
         <v>464</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E119" s="4" t="s">
         <v>565</v>
@@ -8303,7 +8303,7 @@
         <v>464</v>
       </c>
       <c r="D121" s="49" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="E121" s="4" t="s">
         <v>565</v>
@@ -8326,7 +8326,7 @@
         <v>464</v>
       </c>
       <c r="D122" s="49" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="E122" s="4" t="s">
         <v>565</v>
@@ -8349,7 +8349,7 @@
         <v>464</v>
       </c>
       <c r="D123" s="49" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>565</v>
@@ -8372,7 +8372,7 @@
         <v>464</v>
       </c>
       <c r="D124" s="49" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="E124" s="4" t="s">
         <v>565</v>
@@ -8395,7 +8395,7 @@
         <v>464</v>
       </c>
       <c r="D125" s="49" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>565</v>
@@ -8418,7 +8418,7 @@
         <v>464</v>
       </c>
       <c r="D126" s="49" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E126" s="4" t="s">
         <v>565</v>
@@ -8462,7 +8462,7 @@
         <v>464</v>
       </c>
       <c r="D128" s="49" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="E128" s="4" t="s">
         <v>565</v>
@@ -8479,7 +8479,7 @@
         <v>211</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C129" s="24" t="s">
         <v>461</v>
@@ -8506,7 +8506,7 @@
         <v>464</v>
       </c>
       <c r="D130" s="49" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="E130" s="4" t="s">
         <v>565</v>
@@ -8542,7 +8542,7 @@
         <v>444</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C132" s="12"/>
       <c r="D132" s="12"/>
@@ -8561,7 +8561,7 @@
         <v>461</v>
       </c>
       <c r="D133" s="51" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="45">
@@ -8573,7 +8573,7 @@
         <v>464</v>
       </c>
       <c r="D134" s="49" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E134" s="4" t="s">
         <v>690</v>
@@ -8594,7 +8594,7 @@
         <v>464</v>
       </c>
       <c r="D135" s="49" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E135" s="4" t="s">
         <v>690</v>
@@ -8615,7 +8615,7 @@
         <v>464</v>
       </c>
       <c r="D136" s="49" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E136" s="4" t="s">
         <v>690</v>
@@ -8636,7 +8636,7 @@
         <v>464</v>
       </c>
       <c r="D137" s="49" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>690</v>
@@ -8657,7 +8657,7 @@
         <v>464</v>
       </c>
       <c r="D138" s="49" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="E138" s="4" t="s">
         <v>690</v>
@@ -8678,7 +8678,7 @@
         <v>464</v>
       </c>
       <c r="D139" s="49" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>690</v>
@@ -8699,7 +8699,7 @@
         <v>464</v>
       </c>
       <c r="D140" s="49" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E140" s="4" t="s">
         <v>690</v>
@@ -8716,7 +8716,7 @@
         <v>445</v>
       </c>
       <c r="B141" s="12" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C141" s="12"/>
       <c r="D141" s="12"/>
@@ -8735,7 +8735,7 @@
         <v>461</v>
       </c>
       <c r="D142" s="48" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="143" spans="1:7">
@@ -8749,7 +8749,7 @@
         <v>464</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="E143" s="4" t="s">
         <v>9</v>
@@ -8772,7 +8772,7 @@
         <v>464</v>
       </c>
       <c r="D144" s="4" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="E144" s="4" t="s">
         <v>9</v>
@@ -8793,7 +8793,7 @@
         <v>464</v>
       </c>
       <c r="D145" s="4" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E145" s="4" t="s">
         <v>9</v>
@@ -8816,7 +8816,7 @@
         <v>464</v>
       </c>
       <c r="D146" s="4" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E146" s="4" t="s">
         <v>9</v>
@@ -8839,7 +8839,7 @@
         <v>464</v>
       </c>
       <c r="D147" s="4" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E147" s="4" t="s">
         <v>9</v>
@@ -8862,7 +8862,7 @@
         <v>464</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E148" s="4" t="s">
         <v>9</v>
@@ -8879,7 +8879,7 @@
         <v>446</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C149" s="12"/>
       <c r="D149" s="12"/>
@@ -8898,7 +8898,7 @@
         <v>461</v>
       </c>
       <c r="D150" s="55" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="42">
@@ -8912,7 +8912,7 @@
         <v>464</v>
       </c>
       <c r="D151" s="7" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E151" s="4" t="s">
         <v>709</v>
@@ -8935,7 +8935,7 @@
         <v>464</v>
       </c>
       <c r="D152" s="7" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E152" s="4" t="s">
         <v>709</v>
@@ -8970,7 +8970,7 @@
         <v>464</v>
       </c>
       <c r="D154" s="43" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E154" s="4" t="s">
         <v>714</v>
@@ -8993,7 +8993,7 @@
         <v>464</v>
       </c>
       <c r="D155" s="43" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="E155" s="4" t="s">
         <v>714</v>
@@ -9010,7 +9010,7 @@
         <v>11</v>
       </c>
       <c r="B156" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C156" s="12"/>
       <c r="D156" s="12"/>
@@ -9041,7 +9041,7 @@
         <v>464</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E158" s="4" t="s">
         <v>11</v>
@@ -9064,7 +9064,7 @@
         <v>464</v>
       </c>
       <c r="D159" s="20" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="E159" s="4" t="s">
         <v>11</v>
@@ -9087,7 +9087,7 @@
         <v>464</v>
       </c>
       <c r="D160" s="20" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E160" t="s">
         <v>11</v>
@@ -9110,7 +9110,7 @@
         <v>464</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E161" s="4" t="s">
         <v>592</v>
@@ -9133,7 +9133,7 @@
         <v>464</v>
       </c>
       <c r="D162" s="20" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="E162" s="4" t="s">
         <v>592</v>
@@ -9156,7 +9156,7 @@
         <v>464</v>
       </c>
       <c r="D163" s="20" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E163" s="4" t="s">
         <v>592</v>
@@ -9179,7 +9179,7 @@
         <v>464</v>
       </c>
       <c r="D164" s="22" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E164" s="4" t="s">
         <v>592</v>
@@ -9202,7 +9202,7 @@
         <v>464</v>
       </c>
       <c r="D165" s="20" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="E165" s="4" t="s">
         <v>592</v>
@@ -9225,7 +9225,7 @@
         <v>722</v>
       </c>
       <c r="D166" s="33" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="E166" s="4" t="s">
         <v>11</v>
@@ -9248,7 +9248,7 @@
         <v>464</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E167" s="4" t="s">
         <v>11</v>
@@ -9271,7 +9271,7 @@
         <v>464</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E168" s="4" t="s">
         <v>11</v>
@@ -9294,7 +9294,7 @@
         <v>464</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E169" s="4" t="s">
         <v>11</v>
@@ -9317,7 +9317,7 @@
         <v>464</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E170" s="4" t="s">
         <v>11</v>
@@ -9340,7 +9340,7 @@
         <v>464</v>
       </c>
       <c r="D171" s="49" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="E171" s="4" t="s">
         <v>11</v>
@@ -9363,7 +9363,7 @@
         <v>464</v>
       </c>
       <c r="D172" s="49" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E172" s="4" t="s">
         <v>11</v>
@@ -9386,7 +9386,7 @@
         <v>464</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="E173" s="4" t="s">
         <v>11</v>
@@ -9409,7 +9409,7 @@
         <v>464</v>
       </c>
       <c r="D174" s="20" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E174" s="4" t="s">
         <v>11</v>
@@ -9432,7 +9432,7 @@
         <v>464</v>
       </c>
       <c r="D175" s="20" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E175" s="4" t="s">
         <v>11</v>
@@ -9455,7 +9455,7 @@
         <v>464</v>
       </c>
       <c r="D176" s="20" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="E176" s="4" t="s">
         <v>11</v>
@@ -9478,7 +9478,7 @@
         <v>464</v>
       </c>
       <c r="D177" s="20" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E177" s="4" t="s">
         <v>11</v>
@@ -9501,7 +9501,7 @@
         <v>464</v>
       </c>
       <c r="D178" s="20" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E178" s="4" t="s">
         <v>11</v>
@@ -9524,7 +9524,7 @@
         <v>464</v>
       </c>
       <c r="D179" s="20" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E179" s="4" t="s">
         <v>11</v>
@@ -9560,7 +9560,7 @@
         <v>468</v>
       </c>
       <c r="B181" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C181" s="12"/>
       <c r="D181" s="12"/>
@@ -9579,7 +9579,7 @@
         <v>464</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="E182" s="4" t="s">
         <v>11</v>
@@ -9602,7 +9602,7 @@
         <v>464</v>
       </c>
       <c r="D183" s="49" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E183" s="4" t="s">
         <v>11</v>
@@ -9625,7 +9625,7 @@
         <v>464</v>
       </c>
       <c r="D184" s="49" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E184" s="4" t="s">
         <v>11</v>
@@ -9648,7 +9648,7 @@
         <v>464</v>
       </c>
       <c r="D185" s="49" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="E185" s="4" t="s">
         <v>11</v>
@@ -9665,7 +9665,7 @@
         <v>7</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C186" s="12"/>
       <c r="D186" s="12"/>
@@ -9684,7 +9684,7 @@
         <v>464</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="E187" s="4" t="s">
         <v>7</v>
@@ -9707,7 +9707,7 @@
         <v>464</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E188" s="4" t="s">
         <v>7</v>
@@ -9730,7 +9730,7 @@
         <v>464</v>
       </c>
       <c r="D189" s="2" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E189" s="4" t="s">
         <v>7</v>
@@ -9753,7 +9753,7 @@
         <v>464</v>
       </c>
       <c r="D190" s="18" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E190" s="4" t="s">
         <v>7</v>
@@ -9776,7 +9776,7 @@
         <v>464</v>
       </c>
       <c r="D191" s="6" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E191" s="4" t="s">
         <v>7</v>
@@ -9793,7 +9793,7 @@
         <v>450</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C192" s="12"/>
       <c r="D192" s="12"/>
@@ -9810,7 +9810,7 @@
         <v>464</v>
       </c>
       <c r="D193" s="18" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E193" s="4" t="s">
         <v>592</v>
@@ -9831,7 +9831,7 @@
         <v>464</v>
       </c>
       <c r="D194" s="18" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E194" s="4" t="s">
         <v>592</v>
@@ -9852,7 +9852,7 @@
         <v>464</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E195" s="4" t="s">
         <v>592</v>
@@ -9881,7 +9881,7 @@
         <v>451</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C197" s="12"/>
       <c r="D197" s="12"/>
@@ -9897,10 +9897,10 @@
         <v>95</v>
       </c>
       <c r="C198" s="28" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E198" s="4" t="s">
         <v>592</v>
@@ -9923,7 +9923,7 @@
         <v>464</v>
       </c>
       <c r="D199" s="2" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E199" s="4" t="s">
         <v>592</v>
@@ -9959,10 +9959,10 @@
         <v>324</v>
       </c>
       <c r="B201" s="28" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C201" s="28" t="s">
         <v>1109</v>
-      </c>
-      <c r="C201" s="28" t="s">
-        <v>1110</v>
       </c>
       <c r="D201" s="2"/>
       <c r="E201" s="4" t="s">
@@ -9980,7 +9980,7 @@
         <v>470</v>
       </c>
       <c r="B202" s="12" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C202" s="12"/>
       <c r="D202" s="12"/>
@@ -9999,7 +9999,7 @@
         <v>464</v>
       </c>
       <c r="D203" s="6" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="E203" s="4" t="s">
         <v>565</v>
@@ -10022,7 +10022,7 @@
         <v>464</v>
       </c>
       <c r="D204" s="6" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="E204" s="4" t="s">
         <v>812</v>
@@ -10045,7 +10045,7 @@
         <v>464</v>
       </c>
       <c r="D205" s="18" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="E205" s="4" t="s">
         <v>812</v>
@@ -10068,7 +10068,7 @@
         <v>464</v>
       </c>
       <c r="D206" s="6" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="E206" s="4" t="s">
         <v>812</v>
@@ -10091,7 +10091,7 @@
         <v>464</v>
       </c>
       <c r="D207" s="6" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="E207" s="4" t="s">
         <v>812</v>
@@ -10114,7 +10114,7 @@
         <v>464</v>
       </c>
       <c r="D208" s="6" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="E208" s="4" t="s">
         <v>812</v>
@@ -10131,7 +10131,7 @@
         <v>452</v>
       </c>
       <c r="B209" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C209" s="12"/>
       <c r="D209" s="12"/>
@@ -10148,7 +10148,7 @@
       </c>
       <c r="C210" s="46"/>
       <c r="D210" s="54" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="211" spans="1:7">
@@ -10162,7 +10162,7 @@
         <v>464</v>
       </c>
       <c r="D211" s="6" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="E211" s="4" t="s">
         <v>823</v>
@@ -10185,7 +10185,7 @@
         <v>464</v>
       </c>
       <c r="D212" s="22" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="E212" s="26" t="s">
         <v>823</v>
@@ -10208,7 +10208,7 @@
         <v>464</v>
       </c>
       <c r="D213" s="6" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="E213" s="4" t="s">
         <v>823</v>
@@ -10231,7 +10231,7 @@
         <v>464</v>
       </c>
       <c r="D214" s="6" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="E214" s="4" t="s">
         <v>823</v>
@@ -10248,7 +10248,7 @@
         <v>8</v>
       </c>
       <c r="B215" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C215" s="12"/>
       <c r="D215" s="12"/>
@@ -10267,7 +10267,7 @@
         <v>474</v>
       </c>
       <c r="D216" s="51" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="217" spans="1:7" ht="28">
@@ -10281,7 +10281,7 @@
         <v>464</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="E217" s="4" t="s">
         <v>8</v>
@@ -10304,7 +10304,7 @@
         <v>464</v>
       </c>
       <c r="D218" s="53" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="E218" s="4" t="s">
         <v>8</v>
@@ -10327,7 +10327,7 @@
         <v>464</v>
       </c>
       <c r="D219" s="2" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="E219" s="4" t="s">
         <v>8</v>
@@ -10350,7 +10350,7 @@
         <v>464</v>
       </c>
       <c r="D220" s="2" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="E220" s="4" t="s">
         <v>8</v>
@@ -10367,7 +10367,7 @@
         <v>839</v>
       </c>
       <c r="B221" s="12" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C221" s="12"/>
       <c r="D221" s="12"/>
@@ -10496,7 +10496,7 @@
         <v>852</v>
       </c>
       <c r="B228" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C228" s="12"/>
       <c r="D228" s="12"/>
@@ -10515,7 +10515,7 @@
         <v>461</v>
       </c>
       <c r="D229" s="35" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="230" spans="1:7">
@@ -10567,7 +10567,7 @@
         <v>464</v>
       </c>
       <c r="D232" s="4" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E232" s="4" t="s">
         <v>854</v>
@@ -10590,7 +10590,7 @@
         <v>464</v>
       </c>
       <c r="D233" s="4" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E233" s="4" t="s">
         <v>854</v>
@@ -10613,7 +10613,7 @@
         <v>464</v>
       </c>
       <c r="D234" s="4" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="E234" s="4" t="s">
         <v>854</v>
@@ -10651,7 +10651,7 @@
         <v>348</v>
       </c>
       <c r="B236" s="11" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="C236" s="11"/>
       <c r="D236" s="4"/>
@@ -10670,7 +10670,7 @@
         <v>17</v>
       </c>
       <c r="B237" s="11" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="C237" s="11"/>
       <c r="D237" s="4"/>
@@ -10695,7 +10695,7 @@
         <v>464</v>
       </c>
       <c r="D238" s="4" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="E238" s="4" t="s">
         <v>854</v>
@@ -10712,7 +10712,7 @@
         <v>18</v>
       </c>
       <c r="B239" s="11" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="C239" s="11"/>
       <c r="D239" s="4"/>
@@ -10773,7 +10773,7 @@
         <v>453</v>
       </c>
       <c r="B242" s="12" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C242" s="12"/>
       <c r="D242" s="12"/>
@@ -10811,7 +10811,7 @@
         <v>464</v>
       </c>
       <c r="D244" s="4" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E244" s="4" t="s">
         <v>869</v>
@@ -10834,7 +10834,7 @@
         <v>464</v>
       </c>
       <c r="D245" s="4" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="E245" s="4" t="s">
         <v>869</v>
@@ -10857,7 +10857,7 @@
         <v>464</v>
       </c>
       <c r="D246" s="4" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E246" s="4" t="s">
         <v>869</v>
@@ -11014,7 +11014,7 @@
         <v>454</v>
       </c>
       <c r="B261" s="12" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C261" s="12"/>
       <c r="D261" s="12"/>
@@ -11027,10 +11027,10 @@
         <v>639</v>
       </c>
       <c r="C262" s="38" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="D262" s="48" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="E262" s="34" t="s">
         <v>878</v>
@@ -11074,7 +11074,7 @@
         <v>464</v>
       </c>
       <c r="D264" s="4" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="E264" s="4" t="s">
         <v>878</v>
@@ -11097,7 +11097,7 @@
         <v>464</v>
       </c>
       <c r="D265" s="21" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E265" s="34" t="s">
         <v>878</v>
@@ -11120,7 +11120,7 @@
         <v>464</v>
       </c>
       <c r="D266" s="4" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="E266" s="4" t="s">
         <v>878</v>
@@ -11143,7 +11143,7 @@
         <v>464</v>
       </c>
       <c r="D267" s="20" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E267" s="34" t="s">
         <v>878</v>
@@ -11166,7 +11166,7 @@
         <v>464</v>
       </c>
       <c r="D268" s="17" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E268" s="4" t="s">
         <v>878</v>
@@ -11208,7 +11208,7 @@
         <v>464</v>
       </c>
       <c r="D270" s="21" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="E270" s="34" t="s">
         <v>878</v>
@@ -11250,7 +11250,7 @@
         <v>464</v>
       </c>
       <c r="D272" s="4" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E272" s="4" t="s">
         <v>878</v>
@@ -11273,7 +11273,7 @@
         <v>464</v>
       </c>
       <c r="D273" s="4" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="E273" s="4" t="s">
         <v>878</v>
@@ -11296,7 +11296,7 @@
         <v>464</v>
       </c>
       <c r="D274" s="4" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="E274" s="4" t="s">
         <v>878</v>
@@ -11319,7 +11319,7 @@
         <v>464</v>
       </c>
       <c r="D275" s="4" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="E275" s="4" t="s">
         <v>878</v>
@@ -11336,7 +11336,7 @@
         <v>19</v>
       </c>
       <c r="B276" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C276" s="12"/>
       <c r="D276" s="12"/>
@@ -11393,7 +11393,7 @@
         <v>464</v>
       </c>
       <c r="D279" s="4" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="E279" s="4" t="s">
         <v>904</v>
@@ -11530,7 +11530,7 @@
         <v>464</v>
       </c>
       <c r="D286" s="22" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="E286" s="34" t="s">
         <v>904</v>
@@ -11566,7 +11566,7 @@
         <v>455</v>
       </c>
       <c r="B288" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C288" s="12"/>
       <c r="D288" s="12"/>
@@ -11585,7 +11585,7 @@
         <v>464</v>
       </c>
       <c r="D289" s="4" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="E289" s="4" t="s">
         <v>929</v>
@@ -11627,7 +11627,7 @@
         <v>464</v>
       </c>
       <c r="D291" s="4" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="E291" s="4" t="s">
         <v>929</v>
@@ -11650,7 +11650,7 @@
         <v>464</v>
       </c>
       <c r="D292" s="4" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="E292" s="4" t="s">
         <v>929</v>
@@ -11667,13 +11667,13 @@
         <v>418</v>
       </c>
       <c r="B293" s="22" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C293" s="22" t="s">
         <v>464</v>
       </c>
       <c r="D293" s="22" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E293" s="34" t="s">
         <v>929</v>
@@ -11690,13 +11690,13 @@
         <v>419</v>
       </c>
       <c r="B294" s="22" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C294" s="22" t="s">
         <v>464</v>
       </c>
       <c r="D294" s="22" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E294" s="34" t="s">
         <v>929</v>
@@ -11713,13 +11713,13 @@
         <v>420</v>
       </c>
       <c r="B295" s="22" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="C295" s="22" t="s">
         <v>464</v>
       </c>
       <c r="D295" s="22" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E295" s="34" t="s">
         <v>929</v>
@@ -11742,7 +11742,7 @@
         <v>464</v>
       </c>
       <c r="D296" s="4" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E296" s="4" t="s">
         <v>929</v>
@@ -11759,13 +11759,13 @@
         <v>423</v>
       </c>
       <c r="B297" s="22" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="C297" s="22" t="s">
         <v>464</v>
       </c>
       <c r="D297" s="22" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="E297" s="34" t="s">
         <v>929</v>
@@ -11782,13 +11782,13 @@
         <v>422</v>
       </c>
       <c r="B298" s="22" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C298" s="22" t="s">
         <v>464</v>
       </c>
       <c r="D298" s="22" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="E298" s="34" t="s">
         <v>929</v>
@@ -11811,7 +11811,7 @@
         <v>464</v>
       </c>
       <c r="D299" s="4" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="E299" s="4" t="s">
         <v>929</v>
@@ -11828,7 +11828,7 @@
         <v>456</v>
       </c>
       <c r="B300" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C300" s="12"/>
       <c r="D300" s="12"/>
@@ -11866,7 +11866,7 @@
         <v>464</v>
       </c>
       <c r="D302" s="4" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="E302" s="4" t="s">
         <v>950</v>
@@ -11883,13 +11883,13 @@
         <v>433</v>
       </c>
       <c r="B303" s="4" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="C303" s="4" t="s">
         <v>464</v>
       </c>
       <c r="D303" s="4" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E303" s="4" t="s">
         <v>950</v>
@@ -11906,7 +11906,7 @@
         <v>457</v>
       </c>
       <c r="B304" s="12" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C304" s="12"/>
       <c r="D304" s="12"/>
@@ -11940,7 +11940,7 @@
         <v>464</v>
       </c>
       <c r="D306" s="22" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="E306" s="34" t="s">
         <v>950</v>
@@ -11978,7 +11978,7 @@
         <v>464</v>
       </c>
       <c r="D308" s="22" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E308" s="34" t="s">
         <v>950</v>

</xml_diff>